<commit_message>
fixed conflictos de librerias y rutas
</commit_message>
<xml_diff>
--- a/src/empleados.xlsx
+++ b/src/empleados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rody\ia_pruebas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RoseWT\Documents\TF-PromptCTEC\Programa\TF-Prompting-Cybertec\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA004A55-8C78-4034-ADF1-F333070A0E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90007EBF-56C3-4FD6-81B2-2733C06EE604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>ID</t>
   </si>
@@ -79,13 +79,16 @@
   </si>
   <si>
     <t>dabat74405@regapts.com</t>
+  </si>
+  <si>
+    <t>Edad</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,6 +101,14 @@
       <color rgb="FF374151"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -120,7 +131,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -128,6 +139,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,7 +433,7 @@
     <col min="5" max="5" width="39.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -437,8 +449,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -454,8 +469,11 @@
       <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -471,8 +489,11 @@
       <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -488,8 +509,12 @@
       <c r="E4" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>18</v>
+      </c>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -505,28 +530,31 @@
       <c r="E5" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
     </row>

</xml_diff>

<commit_message>
mod README add requirementes.txt
</commit_message>
<xml_diff>
--- a/src/empleados.xlsx
+++ b/src/empleados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RoseWT\Documents\TF-PromptCTEC\Programa\TF-Prompting-Cybertec\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodyv\CodeProyects\CbtecProyects\GPTAutoMail\GPTAutoMail\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409757FA-E87B-4B75-AAF8-A9E9CB94E720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{392899CA-2D01-44DD-AA8C-CC7B099DE453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16560" yWindow="9015" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
   <si>
     <t>ID</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>gotamih382@grassdev.com</t>
+  </si>
+  <si>
+    <t>najehem516@mcuma.com</t>
   </si>
 </sst>
 </file>
@@ -252,7 +255,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -262,6 +265,12 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -546,7 +555,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,7 +581,7 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
       <c r="F1" t="s">
@@ -596,9 +605,9 @@
         <v>23</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>38</v>
       </c>
       <c r="F2">
@@ -622,9 +631,9 @@
         <v>24</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>39</v>
       </c>
       <c r="F3">
@@ -650,7 +659,7 @@
       <c r="D4" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F4">
@@ -676,7 +685,7 @@
       <c r="D5" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="5" t="s">
         <v>41</v>
       </c>
       <c r="F5">
@@ -702,7 +711,7 @@
       <c r="D6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="6" t="s">
         <v>42</v>
       </c>
       <c r="F6">
@@ -728,7 +737,7 @@
       <c r="D7" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="6" t="s">
         <v>43</v>
       </c>
       <c r="F7">
@@ -754,7 +763,7 @@
       <c r="D8" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="6" t="s">
         <v>44</v>
       </c>
       <c r="F8">
@@ -780,7 +789,7 @@
       <c r="D9" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="6" t="s">
         <v>45</v>
       </c>
       <c r="F9">
@@ -806,7 +815,7 @@
       <c r="D10" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="6" t="s">
         <v>46</v>
       </c>
       <c r="F10">
@@ -832,7 +841,7 @@
       <c r="D11" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="6" t="s">
         <v>47</v>
       </c>
       <c r="F11">
@@ -858,7 +867,7 @@
       <c r="D12" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="6" t="s">
         <v>48</v>
       </c>
       <c r="F12">
@@ -884,7 +893,7 @@
       <c r="D13" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="6" t="s">
         <v>49</v>
       </c>
       <c r="F13">
@@ -910,7 +919,7 @@
       <c r="D14" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="6" t="s">
         <v>50</v>
       </c>
       <c r="F14">
@@ -936,7 +945,7 @@
       <c r="D15" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="6" t="s">
         <v>51</v>
       </c>
       <c r="F15">
@@ -962,7 +971,7 @@
       <c r="D16" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="6" t="s">
         <v>52</v>
       </c>
       <c r="F16">

</xml_diff>